<commit_message>
Commit - Desktop Lab, 05/07/2024 as 18:41h.
</commit_message>
<xml_diff>
--- a/out/tabelDadosExperimentais.xlsx
+++ b/out/tabelDadosExperimentais.xlsx
@@ -21,16 +21,16 @@
     <t>DP X (mm)</t>
   </si>
   <si>
+    <t>Resíduo Min X (mm)</t>
+  </si>
+  <si>
+    <t>Resíduo Max X (mm)</t>
+  </si>
+  <si>
     <t>DP Z (mm)</t>
   </si>
   <si>
-    <t>Resíduo Min X (mm)</t>
-  </si>
-  <si>
     <t>Resíduo Min Z (mm)</t>
-  </si>
-  <si>
-    <t>Resíduo Max X (mm)</t>
   </si>
   <si>
     <t>Resíduo Max Z (mm)</t>
@@ -84,10 +84,10 @@
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="true"/>
     <col min="2" max="2" width="10.42578125" customWidth="true"/>
-    <col min="3" max="3" width="10.28515625" customWidth="true"/>
-    <col min="4" max="4" width="18.85546875" customWidth="true"/>
-    <col min="5" max="5" width="18.7109375" customWidth="true"/>
-    <col min="6" max="6" width="19.140625" customWidth="true"/>
+    <col min="3" max="3" width="18.85546875" customWidth="true"/>
+    <col min="4" max="4" width="19.140625" customWidth="true"/>
+    <col min="5" max="5" width="10.28515625" customWidth="true"/>
+    <col min="6" max="6" width="18.7109375" customWidth="true"/>
     <col min="7" max="7" width="19" customWidth="true"/>
   </cols>
   <sheetData>
@@ -119,22 +119,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="0">
-        <v>0.10000000000000001</v>
+        <v>0.080000000000000002</v>
       </c>
       <c r="C2" s="0">
-        <v>0.5</v>
+        <v>-0.20999999999999999</v>
       </c>
       <c r="D2" s="0">
-        <v>-0.40000000000000002</v>
+        <v>0.14999999999999999</v>
       </c>
       <c r="E2" s="0">
-        <v>1.5</v>
+        <v>0.33000000000000002</v>
       </c>
       <c r="F2" s="0">
-        <v>0.40000000000000002</v>
+        <v>-1.0700000000000001</v>
       </c>
       <c r="G2" s="0">
-        <v>-1.6000000000000001</v>
+        <v>1.0800000000000001</v>
       </c>
     </row>
     <row r="3">
@@ -142,22 +142,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="0">
-        <v>0.29999999999999999</v>
+        <v>0.14999999999999999</v>
       </c>
       <c r="C3" s="0">
-        <v>1.3</v>
+        <v>-0.40000000000000002</v>
       </c>
       <c r="D3" s="0">
-        <v>-0.69999999999999996</v>
+        <v>0.31</v>
       </c>
       <c r="E3" s="0">
-        <v>3.8999999999999999</v>
+        <v>0.88</v>
       </c>
       <c r="F3" s="0">
-        <v>0.80000000000000004</v>
+        <v>-2.23</v>
       </c>
       <c r="G3" s="0">
-        <v>-3.2999999999999998</v>
+        <v>2.3900000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -165,22 +165,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="0">
-        <v>0.40000000000000002</v>
+        <v>0.23000000000000001</v>
       </c>
       <c r="C4" s="0">
-        <v>2.6000000000000001</v>
+        <v>-0.58999999999999997</v>
       </c>
       <c r="D4" s="0">
-        <v>-1.2</v>
+        <v>0.46000000000000002</v>
       </c>
       <c r="E4" s="0">
-        <v>8.1999999999999993</v>
+        <v>1.1699999999999999</v>
       </c>
       <c r="F4" s="0">
-        <v>1.1000000000000001</v>
+        <v>-3.8799999999999999</v>
       </c>
       <c r="G4" s="0">
-        <v>-7.2999999999999998</v>
+        <v>3.3300000000000001</v>
       </c>
     </row>
     <row r="5">
@@ -188,22 +188,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="0">
-        <v>0.5</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="C5" s="0">
-        <v>4.9000000000000004</v>
+        <v>-0.76000000000000001</v>
       </c>
       <c r="D5" s="0">
-        <v>-1.5</v>
+        <v>0.63</v>
       </c>
       <c r="E5" s="0">
-        <v>14.800000000000001</v>
+        <v>3.1699999999999999</v>
       </c>
       <c r="F5" s="0">
-        <v>2.2999999999999998</v>
+        <v>-7.3799999999999999</v>
       </c>
       <c r="G5" s="0">
-        <v>-12.9</v>
+        <v>8.4299999999999997</v>
       </c>
     </row>
     <row r="6">
@@ -211,22 +211,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="0">
-        <v>0.59999999999999998</v>
+        <v>0.35999999999999999</v>
       </c>
       <c r="C6" s="0">
-        <v>7.0999999999999996</v>
+        <v>-1.03</v>
       </c>
       <c r="D6" s="0">
-        <v>-1.7</v>
+        <v>0.79000000000000004</v>
       </c>
       <c r="E6" s="0">
-        <v>21</v>
+        <v>3.2599999999999998</v>
       </c>
       <c r="F6" s="0">
-        <v>1.8</v>
+        <v>-9.9900000000000002</v>
       </c>
       <c r="G6" s="0">
-        <v>-19.300000000000001</v>
+        <v>12.640000000000001</v>
       </c>
     </row>
     <row r="7">
@@ -234,22 +234,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="0">
-        <v>0.80000000000000004</v>
+        <v>0.42999999999999999</v>
       </c>
       <c r="C7" s="0">
-        <v>10.800000000000001</v>
+        <v>-1.1299999999999999</v>
       </c>
       <c r="D7" s="0">
-        <v>-2.3999999999999999</v>
+        <v>0.95999999999999996</v>
       </c>
       <c r="E7" s="0">
-        <v>36.5</v>
+        <v>5.54</v>
       </c>
       <c r="F7" s="0">
-        <v>1.7</v>
+        <v>-17.07</v>
       </c>
       <c r="G7" s="0">
-        <v>-29.300000000000001</v>
+        <v>16.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>